<commit_message>
5 consultas hacia las tablas de la base de datos
</commit_message>
<xml_diff>
--- a/cursos.xlsx
+++ b/cursos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,50 +436,109 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>idCurso</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>nombreDescriptivo</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>nAsignaturas</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>nombreDescriptivo</t>
-        </is>
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Programación</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>nombreDescriptivo</t>
-        </is>
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Primero</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>nombreDescriptivo</t>
-        </is>
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Segundo</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>nombreDescriptivo</t>
-        </is>
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Tercero</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>nombreDescriptivo</t>
-        </is>
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Cuarto</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>nombreDescriptivo</t>
-        </is>
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Master</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Doctorado</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>